<commit_message>
ready for first publish
</commit_message>
<xml_diff>
--- a/docs/hardware/Helmoro_BoM_generative_parts.xlsx
+++ b/docs/hardware/Helmoro_BoM_generative_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHE\Documents\Git_Data\HelMoRo\docs\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1363BF8-4B6C-4742-BBED-E73222E5C77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39FB630-A980-45DE-9FFA-E11B6E9B036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>QTY</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>HEL-04-04000-00</t>
-  </si>
-  <si>
-    <t>Generative process</t>
   </si>
   <si>
     <t>HEL-04-04001-00</t>
@@ -4758,7 +4755,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4777,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -5020,51 +5017,57 @@
         <v>50</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -7507,7 +7510,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06A5045-88F5-468D-850B-EA9E68885A27}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F3564D-5489-4EC6-B684-3B78BA1312C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="HelblingDocs"/>

</xml_diff>